<commit_message>
add Generator and Shunt
</commit_message>
<xml_diff>
--- a/Files/nodes_branches.xlsx
+++ b/Files/nodes_branches.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28740" windowHeight="8832"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28740" windowHeight="8832" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="node" sheetId="2" r:id="rId1"/>
     <sheet name="branch" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,81 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="66">
   <si>
-    <t>ВЛ 220 кВ Печора – Северная</t>
-  </si>
-  <si>
-    <t>ВЛ 220 кВ Усинская - КС УГПЗ (ВЛ-249)</t>
-  </si>
-  <si>
-    <t>ВЛ 220 кВ Усинская - КС УГПЗ (ВЛ-250)</t>
-  </si>
-  <si>
-    <t>ВЛ 220 кВ Печорская ГРЭС – Северная</t>
-  </si>
-  <si>
-    <t>ВЛ 220 кВ Ухта – Микунь</t>
-  </si>
-  <si>
-    <t>ВЛ 220 кВ Ухта – Синдор</t>
-  </si>
-  <si>
-    <t>ВЛ 220 кВ Печорская ГРЭС – Инта</t>
-  </si>
-  <si>
-    <t>ВЛ 220 кВ Микунь – Синдор</t>
-  </si>
-  <si>
-    <t>ВЛ 220 кВ Усинская - Промысловая I цепь (ВЛ-253)</t>
-  </si>
-  <si>
-    <t>ВЛ 220 кВ Инта –  Воркута</t>
-  </si>
-  <si>
-    <t>ВЛ 220 кВ Микунь – Урдома</t>
-  </si>
-  <si>
-    <t>ВЛ 220 кВ  Печорская ГРЭС – Печора № 1</t>
-  </si>
-  <si>
-    <t>ВЛ 220 кВ  Печорская ГРЭС - Печора № 2</t>
-  </si>
-  <si>
-    <t>ВЛ 220 кВ Печорская ГРЭС – Зеленоборск</t>
-  </si>
-  <si>
-    <t>ВЛ 220 кВ Печора – Усинская с отпайкой на ПС Сыня</t>
-  </si>
-  <si>
-    <t>ВЛ 220 кВ Ухта – Зеленоборск</t>
-  </si>
-  <si>
-    <t>ВЛ 220 кВ Усинская – Газлифт</t>
-  </si>
-  <si>
-    <t>ВЛ 220 кВ Северный Возей – Харьягинская №2 (ВЛ-282)</t>
-  </si>
-  <si>
-    <t>ВЛ 220 кВ Северный Возей – Харьягинская №1 (ВЛ-283)</t>
-  </si>
-  <si>
-    <t>ВЛ 220 кВ Газлифт– Северный Возей</t>
-  </si>
-  <si>
-    <t>ВЛ 220 кВ Возейская – Северный Возей</t>
-  </si>
-  <si>
-    <t>ВЛ 220 кВ Усинская – Возейская</t>
-  </si>
-  <si>
-    <t>ВЛ 220 кВ Печорская ГРЭС – Усинская с отпайкой на ПС Сыня</t>
-  </si>
-  <si>
-    <t>ВЛ 220 кв Усинская – Промысловая II цепь (ВЛ-254)</t>
-  </si>
-  <si>
-    <t>ВЛ 220 кВ Печорская ГРЭС – Усинская с отпайкой на ПС  Сыня</t>
-  </si>
-  <si>
     <t>ПС 220 кВ Урдома</t>
   </si>
   <si>
@@ -223,6 +148,81 @@
   </si>
   <si>
     <t>qmax</t>
+  </si>
+  <si>
+    <t>ПС 220 кВ Печора - ПС Северная Т-2</t>
+  </si>
+  <si>
+    <t>ПС 220 кВ Усинская - ПС 220 кВ КС УГПЗ</t>
+  </si>
+  <si>
+    <t>Печорская ГРЭС - ПС Северная Т-1</t>
+  </si>
+  <si>
+    <t>ПС 220 кВ Ухта - ПС 220 кВ Микунь</t>
+  </si>
+  <si>
+    <t>ПС 220 кВ Синдор - ПС 220 кВ Ухта</t>
+  </si>
+  <si>
+    <t>Печорская ГРЭС - ПС 220 кВ Инта</t>
+  </si>
+  <si>
+    <t>ПС 220 кВ Микунь - ПС 220 кВ Синдор</t>
+  </si>
+  <si>
+    <t>ПС 220 кВ Усинская - 1c-220 Промысловая</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ПС 220 кВ Инта - ПС 220 кВ Воркута </t>
+  </si>
+  <si>
+    <t>ПС 220 кВ Урдома - ПС 220 кВ Микунь</t>
+  </si>
+  <si>
+    <t>Печорская ГРЭС - ПС 220 кВ Печора</t>
+  </si>
+  <si>
+    <t>ПС 220 кВ Зеленоборск - Печорская ГРЭС</t>
+  </si>
+  <si>
+    <t>ПС 220 кВ Печора - отп. на ПС Сыня-Т1</t>
+  </si>
+  <si>
+    <t>отп. на ПС Сыня-Т1 - ПС 220 кВ Усинская</t>
+  </si>
+  <si>
+    <t>ПС 220 кВ Ухта - ПС 220 кВ Зеленоборск</t>
+  </si>
+  <si>
+    <t>ПС 220 кВ Усинская - ПС 220 кВ Газлифт</t>
+  </si>
+  <si>
+    <t>ПС 220 кВ Харьягинская  - ПС 220 кВ Северный Возей</t>
+  </si>
+  <si>
+    <t>ПС 220 кВ Северный Возей - ПС 220 кВ Газлифт</t>
+  </si>
+  <si>
+    <t>ПС 220 кВ Возейская - ПС 220 кВ Северный Возей</t>
+  </si>
+  <si>
+    <t>ПС 220 кВ Усинская - ПС 220 кВ Возейская</t>
+  </si>
+  <si>
+    <t>Печорская ГРЭС - отп. на ПС Сыня-Т2</t>
+  </si>
+  <si>
+    <t>ПС 220 кВ Усинская - ПС 220 кВ Промысловая</t>
+  </si>
+  <si>
+    <t>отп. на ПС Сыня-Т2 - ПС 220 кВ Сыня-Т2</t>
+  </si>
+  <si>
+    <t>отп. на ПС Сыня-Т1 - ПС 220 кВ Сыня-Т1</t>
+  </si>
+  <si>
+    <t>отп. на ПС Сыня-Т2 - ПС 220 кВ Усинская</t>
   </si>
 </sst>
 </file>
@@ -541,10 +541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L28"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -554,98 +554,101 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="B1" t="s">
-        <v>53</v>
+        <v>28</v>
       </c>
       <c r="C1" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="D1" t="s">
-        <v>58</v>
+        <v>33</v>
       </c>
       <c r="E1" t="s">
-        <v>57</v>
+        <v>32</v>
       </c>
       <c r="F1" t="s">
-        <v>59</v>
+        <v>34</v>
       </c>
       <c r="G1" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="H1" t="s">
-        <v>61</v>
+        <v>36</v>
       </c>
       <c r="I1" t="s">
-        <v>62</v>
+        <v>37</v>
       </c>
       <c r="J1" t="s">
-        <v>63</v>
+        <v>38</v>
       </c>
       <c r="K1" t="s">
-        <v>64</v>
+        <v>39</v>
       </c>
       <c r="L1" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="C2">
         <v>220</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E2">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H2">
-        <v>130.78570455782599</v>
+        <v>0</v>
       </c>
       <c r="I2">
-        <v>-17.732632030805</v>
+        <v>0</v>
       </c>
       <c r="J2">
-        <v>225.3</v>
+        <v>0</v>
       </c>
       <c r="K2">
-        <v>-1000</v>
+        <v>0</v>
       </c>
       <c r="L2">
-        <v>1000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>10</v>
+        <v>89</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
       </c>
       <c r="C3">
         <v>220</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E3">
         <v>409</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -665,25 +668,25 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="C4">
         <v>220</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E4">
         <v>409</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -703,25 +706,25 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="C5">
         <v>220</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E5">
         <v>409</v>
       </c>
       <c r="F5">
-        <v>2.6941583025670899</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>1.29242683141865</v>
+        <v>0</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -741,25 +744,25 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>52</v>
+        <v>88</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="C6">
         <v>220</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E6">
         <v>409</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -779,25 +782,25 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>54</v>
+        <v>131</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C7">
         <v>220</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E7">
         <v>409</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -817,19 +820,19 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>55</v>
+        <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="C8">
         <v>220</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E8">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -838,42 +841,42 @@
         <v>0</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>213.41847225688099</v>
       </c>
       <c r="I8">
-        <v>0</v>
+        <v>-22.489982574081601</v>
       </c>
       <c r="J8">
-        <v>0</v>
+        <v>225.3</v>
       </c>
       <c r="K8">
-        <v>0</v>
+        <v>-9999</v>
       </c>
       <c r="L8">
-        <v>0</v>
+        <v>9999</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="C9">
         <v>220</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E9">
         <v>409</v>
       </c>
       <c r="F9">
-        <v>1.4684145196690199</v>
+        <v>0</v>
       </c>
       <c r="G9">
-        <v>-0.23627137818590399</v>
+        <v>0</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -893,25 +896,25 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>57</v>
+        <v>127</v>
       </c>
       <c r="B10" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="C10">
         <v>220</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E10">
         <v>409</v>
       </c>
       <c r="F10">
-        <v>0.94345165765829797</v>
+        <v>0</v>
       </c>
       <c r="G10">
-        <v>-0.12265239225708401</v>
+        <v>0</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -931,25 +934,25 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="C11">
         <v>220</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E11">
         <v>409</v>
       </c>
       <c r="F11">
-        <v>19.2960050919663</v>
+        <v>0</v>
       </c>
       <c r="G11">
-        <v>4.4824809440748403</v>
+        <v>0</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -969,25 +972,25 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>62</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="C12">
         <v>220</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E12">
         <v>409</v>
       </c>
       <c r="F12">
-        <v>2.6522417141311001</v>
+        <v>0</v>
       </c>
       <c r="G12">
-        <v>-1.88133243383938</v>
+        <v>0</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -1007,25 +1010,25 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="C13">
         <v>220</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E13">
         <v>409</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="G13">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -1045,25 +1048,25 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>66</v>
+        <v>90</v>
       </c>
       <c r="B14" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="C14">
         <v>220</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E14">
         <v>409</v>
       </c>
       <c r="F14">
-        <v>18.916418276259201</v>
+        <v>0</v>
       </c>
       <c r="G14">
-        <v>7.3640895566837701</v>
+        <v>0</v>
       </c>
       <c r="H14">
         <v>0</v>
@@ -1083,25 +1086,25 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>67</v>
+        <v>96</v>
       </c>
       <c r="B15" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="C15">
         <v>220</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E15">
         <v>409</v>
       </c>
       <c r="F15">
-        <v>35.46</v>
+        <v>0</v>
       </c>
       <c r="G15">
-        <v>13.64</v>
+        <v>0</v>
       </c>
       <c r="H15">
         <v>0</v>
@@ -1121,25 +1124,25 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B16" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="C16">
         <v>220</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E16">
         <v>409</v>
       </c>
       <c r="F16">
-        <v>11.9760844487238</v>
+        <v>15</v>
       </c>
       <c r="G16">
-        <v>5.9877352651410796</v>
+        <v>2.5</v>
       </c>
       <c r="H16">
         <v>0</v>
@@ -1159,25 +1162,25 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C17">
         <v>220</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E17">
         <v>409</v>
       </c>
       <c r="F17">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="G17">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="H17">
         <v>0</v>
@@ -1197,25 +1200,25 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="B18" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="C18">
         <v>220</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E18">
         <v>409</v>
       </c>
       <c r="F18">
-        <v>13.571999999999999</v>
+        <v>15</v>
       </c>
       <c r="G18">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="H18">
         <v>0</v>
@@ -1235,25 +1238,25 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="B19" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="C19">
         <v>220</v>
       </c>
       <c r="D19">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E19">
         <v>409</v>
       </c>
       <c r="F19">
-        <v>1.0053705349907101</v>
+        <v>15</v>
       </c>
       <c r="G19">
-        <v>0.19217960280781801</v>
+        <v>2.5</v>
       </c>
       <c r="H19">
         <v>0</v>
@@ -1273,25 +1276,25 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>89</v>
+        <v>54</v>
       </c>
       <c r="B20" t="s">
-        <v>43</v>
+        <v>5</v>
       </c>
       <c r="C20">
         <v>220</v>
       </c>
       <c r="D20">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E20">
         <v>409</v>
       </c>
       <c r="F20">
-        <v>1.3011847554918201</v>
+        <v>0</v>
       </c>
       <c r="G20">
-        <v>0.23336321199460899</v>
+        <v>0</v>
       </c>
       <c r="H20">
         <v>0</v>
@@ -1311,16 +1314,16 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>90</v>
+        <v>69</v>
       </c>
       <c r="B21" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="C21">
         <v>220</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E21">
         <v>409</v>
@@ -1349,25 +1352,25 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>96</v>
+        <v>57</v>
       </c>
       <c r="B22" t="s">
-        <v>45</v>
+        <v>8</v>
       </c>
       <c r="C22">
         <v>220</v>
       </c>
       <c r="D22">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E22">
         <v>409</v>
       </c>
       <c r="F22">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="G22">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="H22">
         <v>0</v>
@@ -1387,25 +1390,25 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>127</v>
+        <v>56</v>
       </c>
       <c r="B23" t="s">
-        <v>46</v>
+        <v>7</v>
       </c>
       <c r="C23">
         <v>220</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E23">
         <v>409</v>
       </c>
       <c r="F23">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="G23">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="H23">
         <v>0</v>
@@ -1425,25 +1428,25 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>131</v>
+        <v>55</v>
       </c>
       <c r="B24" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="C24">
         <v>220</v>
       </c>
       <c r="D24">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E24">
         <v>409</v>
       </c>
       <c r="F24">
-        <v>3.1101352886411902</v>
+        <v>0</v>
       </c>
       <c r="G24">
-        <v>1.1556858252651301</v>
+        <v>0</v>
       </c>
       <c r="H24">
         <v>0</v>
@@ -1459,49 +1462,6 @@
       </c>
       <c r="L24">
         <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A26">
-        <v>1</v>
-      </c>
-      <c r="B26">
-        <v>2</v>
-      </c>
-      <c r="C26">
-        <v>3</v>
-      </c>
-      <c r="D26">
-        <v>4</v>
-      </c>
-      <c r="E26">
-        <v>5</v>
-      </c>
-      <c r="F26">
-        <v>6</v>
-      </c>
-      <c r="G26">
-        <v>7</v>
-      </c>
-      <c r="H26">
-        <v>8</v>
-      </c>
-      <c r="I26">
-        <v>9</v>
-      </c>
-      <c r="J26">
-        <v>10</v>
-      </c>
-      <c r="K26">
-        <v>11</v>
-      </c>
-      <c r="L26">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B28" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1513,8 +1473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6:D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1524,25 +1484,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="B1" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="C1" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="D1" t="s">
-        <v>53</v>
+        <v>28</v>
       </c>
       <c r="E1" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="F1" t="s">
-        <v>49</v>
+        <v>24</v>
       </c>
       <c r="G1" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -1556,7 +1516,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="E2">
         <v>0.29199999999999998</v>
@@ -1579,7 +1539,7 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>1</v>
+        <v>42</v>
       </c>
       <c r="E3">
         <v>0.13</v>
@@ -1602,7 +1562,7 @@
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>2</v>
+        <v>42</v>
       </c>
       <c r="E4">
         <v>0.13</v>
@@ -1625,7 +1585,7 @@
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>3</v>
+        <v>43</v>
       </c>
       <c r="E5">
         <v>0.99099999999999999</v>
@@ -1648,7 +1608,7 @@
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="E6">
         <v>19.003</v>
@@ -1671,7 +1631,7 @@
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="E7">
         <v>14.590999999999999</v>
@@ -1694,16 +1654,16 @@
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="E8">
-        <v>19.181999999999999</v>
+        <v>4.8540000000000001</v>
       </c>
       <c r="F8">
-        <v>76.197999999999993</v>
+        <v>21.69</v>
       </c>
       <c r="G8">
-        <v>-468.916</v>
+        <v>-133.73099999999999</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -1717,16 +1677,16 @@
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
       <c r="E9">
-        <v>11.837999999999999</v>
+        <v>4.8540000000000001</v>
       </c>
       <c r="F9">
-        <v>47.026000000000003</v>
+        <v>21.69</v>
       </c>
       <c r="G9">
-        <v>-289.39600000000002</v>
+        <v>-133.73099999999999</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -1740,16 +1700,16 @@
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="E10">
-        <v>0.42</v>
+        <v>4.8540000000000001</v>
       </c>
       <c r="F10">
-        <v>1.84</v>
+        <v>21.69</v>
       </c>
       <c r="G10">
-        <v>-11.3</v>
+        <v>-133.73099999999999</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -1763,16 +1723,16 @@
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="E11">
-        <v>26.622</v>
+        <v>4.8540000000000001</v>
       </c>
       <c r="F11">
-        <v>105.748</v>
+        <v>21.69</v>
       </c>
       <c r="G11">
-        <v>-650.76</v>
+        <v>-133.73099999999999</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -1786,16 +1746,16 @@
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="E12">
-        <v>12.94056</v>
+        <v>4.8540000000000001</v>
       </c>
       <c r="F12">
-        <v>51.40278</v>
+        <v>21.69</v>
       </c>
       <c r="G12">
-        <v>-316.32499999999999</v>
+        <v>-133.73099999999999</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -1809,7 +1769,7 @@
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>11</v>
+        <v>51</v>
       </c>
       <c r="E13">
         <v>0.73499999999999999</v>
@@ -1832,7 +1792,7 @@
         <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>12</v>
+        <v>51</v>
       </c>
       <c r="E14">
         <v>0.73799999999999999</v>
@@ -1855,7 +1815,7 @@
         <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="E15">
         <v>13.57</v>
@@ -1878,7 +1838,7 @@
         <v>0</v>
       </c>
       <c r="D16" t="s">
-        <v>14</v>
+        <v>53</v>
       </c>
       <c r="E16">
         <v>4.9870000000000001</v>
@@ -1901,7 +1861,7 @@
         <v>0</v>
       </c>
       <c r="D17" t="s">
-        <v>14</v>
+        <v>54</v>
       </c>
       <c r="E17">
         <v>10.541</v>
@@ -1924,7 +1884,7 @@
         <v>0</v>
       </c>
       <c r="D18" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="E18">
         <v>13.91</v>
@@ -1947,7 +1907,7 @@
         <v>0</v>
       </c>
       <c r="D19" t="s">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="E19">
         <v>4.7039999999999997</v>
@@ -1970,7 +1930,7 @@
         <v>2</v>
       </c>
       <c r="D20" t="s">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="E20">
         <v>5.1260000000000003</v>
@@ -1993,7 +1953,7 @@
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>18</v>
+        <v>57</v>
       </c>
       <c r="E21">
         <v>4.8540000000000001</v>
@@ -2016,7 +1976,7 @@
         <v>0</v>
       </c>
       <c r="D22" t="s">
-        <v>19</v>
+        <v>58</v>
       </c>
       <c r="E22">
         <v>6.468</v>
@@ -2039,7 +1999,7 @@
         <v>0</v>
       </c>
       <c r="D23" t="s">
-        <v>20</v>
+        <v>59</v>
       </c>
       <c r="E23">
         <v>5.5460000000000003</v>
@@ -2062,7 +2022,7 @@
         <v>0</v>
       </c>
       <c r="D24" t="s">
-        <v>21</v>
+        <v>60</v>
       </c>
       <c r="E24">
         <v>5.4169999999999998</v>
@@ -2085,7 +2045,7 @@
         <v>0</v>
       </c>
       <c r="D25" t="s">
-        <v>22</v>
+        <v>61</v>
       </c>
       <c r="E25">
         <v>5.4260000000000002</v>
@@ -2108,7 +2068,7 @@
         <v>2</v>
       </c>
       <c r="D26" t="s">
-        <v>23</v>
+        <v>62</v>
       </c>
       <c r="E26">
         <v>0.42</v>
@@ -2131,7 +2091,7 @@
         <v>0</v>
       </c>
       <c r="D27" t="s">
-        <v>24</v>
+        <v>63</v>
       </c>
       <c r="E27">
         <v>1.9999999552965199E-2</v>
@@ -2154,7 +2114,7 @@
         <v>0</v>
       </c>
       <c r="D28" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="E28">
         <v>2.4E-2</v>
@@ -2177,7 +2137,7 @@
         <v>0</v>
       </c>
       <c r="D29" t="s">
-        <v>22</v>
+        <v>65</v>
       </c>
       <c r="E29">
         <v>10.624000000000001</v>

</xml_diff>